<commit_message>
Tested the columns detector
</commit_message>
<xml_diff>
--- a/backend/uploads/masked_Student_Information.xlsx
+++ b/backend/uploads/masked_Student_Information.xlsx
@@ -517,12 +517,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vGqJD8KQweMin</t>
+          <t>Ali bin Ahmad</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>900101-01-1234</t>
+          <t>qD9PBv5QNbVNcR</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -535,7 +535,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>a7YsjRon3vo</t>
+          <t>012-3456789</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -586,12 +586,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P6ggG0fxYVHVvu0B4</t>
+          <t>Siti binti Aminah</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>920202-02-2345</t>
+          <t>fetLua2MOOClsl</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -604,7 +604,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>LH6He0ajbJE</t>
+          <t>013-4567890</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -655,12 +655,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vqS4w1z7Xe9UK</t>
+          <t>Lim Wei Chong</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>940303-03-3456</t>
+          <t>rtmyXBHhwbnAUG</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -673,7 +673,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ERGzpYNFpP0</t>
+          <t>014-5678901</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -724,12 +724,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>U9fkd9dgMXU</t>
+          <t>Preeti Kaur</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>950404-04-4567</t>
+          <t>QzJaY2L4EyW6Pj</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -742,7 +742,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>vMLnMXyePg9</t>
+          <t>015-6789012</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -793,12 +793,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tS1MdAqPYndYAc</t>
+          <t>Muhammad Hafiz</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>960505-05-5678</t>
+          <t>S6yetJh9pxRYWj</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -811,7 +811,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>aQeq0S9IpvV</t>
+          <t>016-7890123</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -862,12 +862,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>VK6RjMsSSre093</t>
+          <t>Chong Mei Ling</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>970606-06-6789</t>
+          <t>egXGWEqM5w1awC</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>BZE9HLyeQuc</t>
+          <t>017-8901234</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -931,12 +931,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MHGnFKeu</t>
+          <t>Arun Raj</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>980707-07-7890</t>
+          <t>l1wLSXU32WIjUX</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>djvjKo8GSu2</t>
+          <t>018-9012345</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1000,12 +1000,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>QcpdLKhaoJqATcAf</t>
+          <t>Farah binti Zain</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>990808-08-8901</t>
+          <t>M3hvlWW3m3HFAQ</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>YFElbDPieva</t>
+          <t>019-0123456</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1069,12 +1069,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>uDiVkfJh0bS</t>
+          <t>Tan Ah Heng</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>000909-09-9012</t>
+          <t>BTdhIhi0T9f2Pe</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>cETC8YLgKau</t>
+          <t>010-2345678</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1138,12 +1138,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>jsZPFjd0MzJ</t>
+          <t>Anusha Devi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>010101-10-0123</t>
+          <t>eLGzmdMyIrQGkD</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V2NFtbjJ2UO</t>
+          <t>011-3456789</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1207,12 +1207,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ihOkReg9LH</t>
+          <t>Nur Aisyah</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>020202-11-1234</t>
+          <t>1KGdZK7P5UsjsI</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EzjpUDjGOAL</t>
+          <t>012-5678901</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UuqWVc3y1ZQQr</t>
+          <t>Wong Siew Mei</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>030303-12-2345</t>
+          <t>gfAVDdxUVzAJME</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>jqGb0e18yCS</t>
+          <t>013-6789012</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1345,12 +1345,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>9MphM819FJHp</t>
+          <t>Thiru Selvan</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>040404-13-3456</t>
+          <t>rbjLa11L9LiYXn</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>C3Yq0Qkbm4z</t>
+          <t>014-7890123</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1414,12 +1414,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>tS9mc7SEOmMYvKxX</t>
+          <t>Aina binti Razak</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>050505-14-4567</t>
+          <t>Jb4pL17VqHUYuX</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>nEC9pH1fgCo</t>
+          <t>015-8901234</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1483,12 +1483,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3SlEHM0BZXHb</t>
+          <t>Yong Kai Wen</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>060606-15-5678</t>
+          <t>nEbs5LCkAUFVFs</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>efkaeqC8q8d</t>
+          <t>016-9012345</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1552,12 +1552,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>49KucMP37e</t>
+          <t>Hema Latha</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>070707-16-6789</t>
+          <t>i10QF4IzAoCK9V</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>br6PDTsB7UH</t>
+          <t>017-0123456</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1621,12 +1621,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>hIzsj3OvEyWWv</t>
+          <t>Ahmad bin Abu</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>080808-17-7890</t>
+          <t>HOLEs7GWMcEPsr</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>8n6wJj9WcFB</t>
+          <t>018-1234567</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1690,12 +1690,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>k8z6ZfK8</t>
+          <t>Mei Fong</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>090909-18-8901</t>
+          <t>kEkXMZDVFtFqFR</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>pWSLoB5J3MY</t>
+          <t>019-2345678</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1759,12 +1759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>lLCqk2yM3e</t>
+          <t>Raju Kumar</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>101010-19-9012</t>
+          <t>q8GSAAPnlKe5z5</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>hjGraHZRbMu</t>
+          <t>010-3456789</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1828,12 +1828,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>I21RKlEs1NO5F</t>
+          <t>Zainal Abidin</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>111111-20-0123</t>
+          <t>J3ksRMS8g22YGo</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>SiAFqBSS2Ag</t>
+          <t>011-4567890</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1897,12 +1897,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>p4mHKfW3TmfiVd33N</t>
+          <t>Amira binti Latif</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>121212-21-1234</t>
+          <t>s5uro6raKM9eUh</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>a5LC3QiNmbm</t>
+          <t>012-5678901</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1966,12 +1966,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>utQ6bNzHxHM2</t>
+          <t>Chia Wei Han</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>131313-22-2345</t>
+          <t>wS4QiOIScAspiY</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1984,7 +1984,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>g8p2DnwAfyV</t>
+          <t>013-6789012</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2035,12 +2035,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>VuBJ5fBBAGPM</t>
+          <t>Suresh Kumar</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>141414-23-3456</t>
+          <t>1fI0EladmVFdaO</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>9oMIJ2jy84o</t>
+          <t>014-7890123</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2104,12 +2104,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>FraHxQzsdx</t>
+          <t>Norhidayah</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>151515-24-4567</t>
+          <t>2SbIreHqQRIlqm</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4SXVHY1EslF</t>
+          <t>015-8901234</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2173,12 +2173,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>vwupCiN6HdX</t>
+          <t>Lim Wei Hui</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>161616-25-5678</t>
+          <t>OebkWAaJpKgyU8</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>gMDuQsyPUu8</t>
+          <t>016-9012345</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2242,12 +2242,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>arZGjOv7N2</t>
+          <t>Arvind Raj</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>171717-26-6789</t>
+          <t>ntEnbjY3tWLSLU</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>tC78T6F0CgF</t>
+          <t>017-0123456</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2311,12 +2311,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ZwnOVL2F3PW7snQ2</t>
+          <t>Safia binti Noor</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>181818-27-7890</t>
+          <t>nZ9T1Bgcxj9eUw</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>9WRbGjykIxJ</t>
+          <t>018-1234567</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2380,12 +2380,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>iWbKcl6JUrGR</t>
+          <t>Wong Kin Fai</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>191919-28-8901</t>
+          <t>rXWaaeI2vOGrPu</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>i3RG0VypcCU</t>
+          <t>019-2345678</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2449,12 +2449,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>M3V89JWGUB4mbTem</t>
+          <t>Aina binti Osman</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>202020-29-9012</t>
+          <t>NSvTwCID4y1RXQ</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>ud3c3lT9Es6</t>
+          <t>010-3456789</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2518,12 +2518,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NlNsBMH57GiHHO0</t>
+          <t>Kumar Narayanan</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>212121-30-0123</t>
+          <t>ZLv2lnnPXBjjqb</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>ZRSWIoQoV2K</t>
+          <t>011-4567890</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">

</xml_diff>

<commit_message>
Made some changes to ensure a more intuitive user experience
</commit_message>
<xml_diff>
--- a/backend/uploads/masked_Student_Information.xlsx
+++ b/backend/uploads/masked_Student_Information.xlsx
@@ -517,12 +517,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ali bin Ahmad</t>
+          <t>AgqO9cblRGPfP</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>qD9PBv5QNbVNcR</t>
+          <t>Bsq7aTk3WfJVuI</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -586,12 +586,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Siti binti Aminah</t>
+          <t>yB8y2eX4O2B9i3QtP</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>fetLua2MOOClsl</t>
+          <t>0iIB0vgKsd5Uxb</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -655,12 +655,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Lim Wei Chong</t>
+          <t>vnbJytzGhqNDj</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>rtmyXBHhwbnAUG</t>
+          <t>rKxPzTWlZdoIax</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -724,12 +724,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Preeti Kaur</t>
+          <t>eDSVmNZleIZ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>QzJaY2L4EyW6Pj</t>
+          <t>eewBTLbrOdhwAn</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -793,12 +793,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Muhammad Hafiz</t>
+          <t>sCTffQ9abI9uyv</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>S6yetJh9pxRYWj</t>
+          <t>Hu8n2dReuN1W9A</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -862,12 +862,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chong Mei Ling</t>
+          <t>CjNz9WPKDM3slT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>egXGWEqM5w1awC</t>
+          <t>6AMzxTs1dOJ5RE</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -931,12 +931,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Arun Raj</t>
+          <t>RJTxKKNj</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>l1wLSXU32WIjUX</t>
+          <t>TFarAhEFenvDLC</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -1000,12 +1000,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Farah binti Zain</t>
+          <t>XHZ1fSzVomfTu0G8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>M3hvlWW3m3HFAQ</t>
+          <t>ukab36PJ6oBEZg</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1069,12 +1069,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tan Ah Heng</t>
+          <t>aNxBoN23Tjf</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BTdhIhi0T9f2Pe</t>
+          <t>CY6Fj98hfEjNWj</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1138,12 +1138,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anusha Devi</t>
+          <t>2Ktf6aBQzOJ</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>eLGzmdMyIrQGkD</t>
+          <t>Co0zPpgQt18Zos</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1207,12 +1207,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nur Aisyah</t>
+          <t>MuwCUV9brr</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1KGdZK7P5UsjsI</t>
+          <t>an0QXwEdV0nl5g</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1276,12 +1276,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wong Siew Mei</t>
+          <t>KVhMhGZC5J7LB</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>gfAVDdxUVzAJME</t>
+          <t>wzvCPfQ5NYxV0s</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1345,12 +1345,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thiru Selvan</t>
+          <t>9uycMVsKMldi</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>rbjLa11L9LiYXn</t>
+          <t>xc8u97rLz2YJF8</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1414,12 +1414,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aina binti Razak</t>
+          <t>ruLDtOxVAdAeX46I</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jb4pL17VqHUYuX</t>
+          <t>XHuj5xE23l7mYp</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1483,12 +1483,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Yong Kai Wen</t>
+          <t>QyGmJibYcdfq</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>nEbs5LCkAUFVFs</t>
+          <t>X9hnRe9hsmRjEG</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1552,12 +1552,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hema Latha</t>
+          <t>U5ZqMJn230</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>i10QF4IzAoCK9V</t>
+          <t>YqqibHjGZicmw1</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1621,12 +1621,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ahmad bin Abu</t>
+          <t>QhK0CUH1V04VT</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HOLEs7GWMcEPsr</t>
+          <t>2i2kXwwI6jUPWw</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1690,12 +1690,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mei Fong</t>
+          <t>Tb4haWmF</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>kEkXMZDVFtFqFR</t>
+          <t>K0eC7S4JNknY8J</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1759,12 +1759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Raju Kumar</t>
+          <t>w1OppE1NcP</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>q8GSAAPnlKe5z5</t>
+          <t>JvnuFXDNYjKPRM</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1828,12 +1828,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zainal Abidin</t>
+          <t>aoDrfxtjiYc15</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>J3ksRMS8g22YGo</t>
+          <t>FYq9LTLyYLzDwh</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1897,12 +1897,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Amira binti Latif</t>
+          <t>4VPM4BIgPjCmkUyUA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>s5uro6raKM9eUh</t>
+          <t>3gthMNwXQYTQhq</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1966,12 +1966,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chia Wei Han</t>
+          <t>Kmnab49t0K6J</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>wS4QiOIScAspiY</t>
+          <t>2UeON4OjdtG38m</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -2035,12 +2035,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Suresh Kumar</t>
+          <t>1kA5hKs3yFu6</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1fI0EladmVFdaO</t>
+          <t>styRoh1ShbqIkX</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -2104,12 +2104,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Norhidayah</t>
+          <t>dfc5tLnL5l</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2SbIreHqQRIlqm</t>
+          <t>32X1rv92UoW5PV</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2173,12 +2173,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lim Wei Hui</t>
+          <t>alN2QAtmdyV</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OebkWAaJpKgyU8</t>
+          <t>EUqwVXZ7ni9CDH</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2242,12 +2242,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Arvind Raj</t>
+          <t>SqqWoInj8P</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ntEnbjY3tWLSLU</t>
+          <t>COUBuaMliNoHaT</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2311,12 +2311,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Safia binti Noor</t>
+          <t>bCcb6SHybod8imYz</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>nZ9T1Bgcxj9eUw</t>
+          <t>UqigEDaswPoJWf</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2380,12 +2380,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Wong Kin Fai</t>
+          <t>jjmI0Lo4ehAe</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>rXWaaeI2vOGrPu</t>
+          <t>Sa1CiHhAOVD5ev</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2449,12 +2449,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Aina binti Osman</t>
+          <t>9wSmdK7CAa2CQw9A</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NSvTwCID4y1RXQ</t>
+          <t>n5X928UHxGVTmk</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2518,12 +2518,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kumar Narayanan</t>
+          <t>sAEgGqW61qIqhMJ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ZLv2lnnPXBjjqb</t>
+          <t>13cGvrTnAUVSfJ</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">

</xml_diff>

<commit_message>
Made some changes on the styles
</commit_message>
<xml_diff>
--- a/backend/uploads/masked_Student_Information.xlsx
+++ b/backend/uploads/masked_Student_Information.xlsx
@@ -517,12 +517,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AgqO9cblRGPfP</t>
+          <t>cmPGHRQ1wTDgq</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bsq7aTk3WfJVuI</t>
+          <t>Kp5AHtI87wg4HS</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -586,12 +586,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>yB8y2eX4O2B9i3QtP</t>
+          <t>1sfdtwUquf46G2EpF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0iIB0vgKsd5Uxb</t>
+          <t>STLlwP6MZYaNSl</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -655,12 +655,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vnbJytzGhqNDj</t>
+          <t>qli7Mh7TpoLDK</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>rKxPzTWlZdoIax</t>
+          <t>NIWL6MC7MBizI5</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -724,12 +724,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>eDSVmNZleIZ</t>
+          <t>R5UC8Ji2MH2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>eewBTLbrOdhwAn</t>
+          <t>3NsMBQdB6weTK4</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -793,12 +793,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sCTffQ9abI9uyv</t>
+          <t>uhMXbHfO4F6nM1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hu8n2dReuN1W9A</t>
+          <t>vYI7FhNhV4IfZl</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -862,12 +862,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CjNz9WPKDM3slT</t>
+          <t>JZaXoOtKamA0XB</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6AMzxTs1dOJ5RE</t>
+          <t>WFEB3e1p6YDdqd</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -931,12 +931,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RJTxKKNj</t>
+          <t>oS5Y3mDH</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TFarAhEFenvDLC</t>
+          <t>jLdJlrNDcfvWBR</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -1000,12 +1000,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>XHZ1fSzVomfTu0G8</t>
+          <t>A6ojfKtxnVSVu0yx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ukab36PJ6oBEZg</t>
+          <t>MDs6rkWdfkth6E</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1069,12 +1069,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>aNxBoN23Tjf</t>
+          <t>TAwzSy1WpFv</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CY6Fj98hfEjNWj</t>
+          <t>Ca6OGW1Uyiimui</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1138,12 +1138,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2Ktf6aBQzOJ</t>
+          <t>JqS0gfy7vtY</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Co0zPpgQt18Zos</t>
+          <t>paFQ0kNQ7SyOw2</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1207,12 +1207,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MuwCUV9brr</t>
+          <t>N2kcjX08V4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>an0QXwEdV0nl5g</t>
+          <t>G0CJg1UY38Nurr</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1276,12 +1276,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KVhMhGZC5J7LB</t>
+          <t>E9S1RkAB0058V</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>wzvCPfQ5NYxV0s</t>
+          <t>aX6dyXY6QYY1GF</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1345,12 +1345,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>9uycMVsKMldi</t>
+          <t>D6YO4mlxLR2k</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>xc8u97rLz2YJF8</t>
+          <t>uPQQDox8V1d0zi</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1414,12 +1414,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ruLDtOxVAdAeX46I</t>
+          <t>M41K7UOctvFHTozD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>XHuj5xE23l7mYp</t>
+          <t>gsFBZCqCEEtygt</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1483,12 +1483,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>QyGmJibYcdfq</t>
+          <t>26L3mcAf846U</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>X9hnRe9hsmRjEG</t>
+          <t>w9d4HTLRWX43HX</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1552,12 +1552,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>U5ZqMJn230</t>
+          <t>bdoTC2SbVQ</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>YqqibHjGZicmw1</t>
+          <t>hoSxqo1xRSV9RF</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1621,12 +1621,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>QhK0CUH1V04VT</t>
+          <t>OcaK582RDtWqy</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2i2kXwwI6jUPWw</t>
+          <t>cr9a4zpx3ncy7z</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1690,12 +1690,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Tb4haWmF</t>
+          <t>RtisSO5H</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>K0eC7S4JNknY8J</t>
+          <t>2ouVkZ917lDRfL</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1759,12 +1759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>w1OppE1NcP</t>
+          <t>wm6q9pBIEG</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>JvnuFXDNYjKPRM</t>
+          <t>YSxoi8WsjoaL6J</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1828,12 +1828,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>aoDrfxtjiYc15</t>
+          <t>7JRMYIgWEXDA2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>FYq9LTLyYLzDwh</t>
+          <t>7jY1GE7eyJdIQH</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1897,12 +1897,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4VPM4BIgPjCmkUyUA</t>
+          <t>eFQV6r8lSCyWCiAYA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3gthMNwXQYTQhq</t>
+          <t>BQX9bsaqvb0oAT</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -1966,12 +1966,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Kmnab49t0K6J</t>
+          <t>6FL5dmyV4Op6</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2UeON4OjdtG38m</t>
+          <t>ag1AWmKIVHfUnO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -2035,12 +2035,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1kA5hKs3yFu6</t>
+          <t>6woMwPcalVMf</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>styRoh1ShbqIkX</t>
+          <t>4o2Cc451lafM0z</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -2104,12 +2104,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>dfc5tLnL5l</t>
+          <t>qa4LgVOnoh</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>32X1rv92UoW5PV</t>
+          <t>y86ZQh1n8QafBf</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2173,12 +2173,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>alN2QAtmdyV</t>
+          <t>7FN5cCajm6F</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>EUqwVXZ7ni9CDH</t>
+          <t>KGuYiLtJWMyoci</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2242,12 +2242,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SqqWoInj8P</t>
+          <t>0mrf1jjnZs</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>COUBuaMliNoHaT</t>
+          <t>QVcNGK2kyt3dgw</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2311,12 +2311,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bCcb6SHybod8imYz</t>
+          <t>aOiV6DchmlyehaQl</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>UqigEDaswPoJWf</t>
+          <t>fmHVtX5png1c7E</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2380,12 +2380,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>jjmI0Lo4ehAe</t>
+          <t>z5D3gzhIEeiZ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sa1CiHhAOVD5ev</t>
+          <t>fF8uY9p2Ynf1xm</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2449,12 +2449,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>9wSmdK7CAa2CQw9A</t>
+          <t>JFYjrSlWpOUXY8fA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>n5X928UHxGVTmk</t>
+          <t>8h3J8DZw1XppT6</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2518,12 +2518,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>sAEgGqW61qIqhMJ</t>
+          <t>LhdmFJxyJwmAgzq</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>13cGvrTnAUVSfJ</t>
+          <t>9n16ddjwGPOjxW</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">

</xml_diff>